<commit_message>
add new dataSets, better start with csript ....
</commit_message>
<xml_diff>
--- a/sourceData.xlsx
+++ b/sourceData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herci\Desktop\OS2\semestrlka\semOS2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67422A08-8D73-4719-BFB6-19B5E28ED172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA62AE8F-283F-47E5-9D5B-CDAFED69D2DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B0CC420B-97CC-46EA-9B55-E964C6A1DA68}"/>
   </bookViews>
@@ -33,26 +33,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>WindowsProductName</t>
   </si>
   <si>
-    <t>WindowsCurrentVersion</t>
-  </si>
-  <si>
     <t>WindowsVersion</t>
   </si>
   <si>
     <t>BiosManufacturer</t>
   </si>
   <si>
-    <t>BiosName</t>
-  </si>
-  <si>
-    <t>BiosSeralNumber</t>
-  </si>
-  <si>
     <t>CsDNSHostName</t>
   </si>
   <si>
@@ -65,13 +56,25 @@
     <t>OsArchitecture</t>
   </si>
   <si>
-    <t xml:space="preserve"> Get-ComputerInfo</t>
-  </si>
-  <si>
-    <t>systeminfo</t>
-  </si>
-  <si>
     <t>Hotfix(s)</t>
+  </si>
+  <si>
+    <t>Windows 10 Home</t>
+  </si>
+  <si>
+    <t>Dell Inc.</t>
+  </si>
+  <si>
+    <t>DESKTOP-SQSHR1A</t>
+  </si>
+  <si>
+    <t>WORKGROUP</t>
+  </si>
+  <si>
+    <t>64bitový</t>
+  </si>
+  <si>
+    <t>KB5012117</t>
   </si>
 </sst>
 </file>
@@ -424,71 +427,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5089DAD5-A6E0-4257-91A6-C93611A18307}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>2009</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
+      <c r="F2">
+        <v>16671872</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>